<commit_message>
Enhance article import process by adding detailed success response and new functions for opercule, couvercle, coiffe, and carton information retrieval
</commit_message>
<xml_diff>
--- a/RESSOURCES/EMBALLAGES PAR PRODUITS TTES MARQUES.xlsx
+++ b/RESSOURCES/EMBALLAGES PAR PRODUITS TTES MARQUES.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CLAIRE\ACHATS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\econte\Desktop\Edouard\Divisio\RESSOURCES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C437B710-1197-4FBC-93A7-9A3EC28D9828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B0E9F0-0828-4BE5-9BE7-49F51191D27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{CE562C63-56AB-4767-B83C-50F8A455B02C}"/>
   </bookViews>
@@ -10710,16 +10710,16 @@
   </sheetData>
   <autoFilter ref="J3:J18" xr:uid="{8FF0F9D2-17B0-4D09-9DF1-2E903DE4C1A8}"/>
   <mergeCells count="10">
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AO2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="U2:X2"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="U2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" fitToWidth="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -13514,11 +13514,11 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="K4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="O4" sqref="O4"/>
       <selection pane="topRight" activeCell="O4" sqref="O4"/>
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add fournisseur routes and services, enhance article service with relation establishment, and update schemas for better data handling
</commit_message>
<xml_diff>
--- a/RESSOURCES/EMBALLAGES PAR PRODUITS TTES MARQUES.xlsx
+++ b/RESSOURCES/EMBALLAGES PAR PRODUITS TTES MARQUES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\econte\Desktop\Edouard\Divisio\RESSOURCES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B0E9F0-0828-4BE5-9BE7-49F51191D27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367F2248-C3D9-4C2A-ACC0-5B57B79E029C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{CE562C63-56AB-4767-B83C-50F8A455B02C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE562C63-56AB-4767-B83C-50F8A455B02C}"/>
   </bookViews>
   <sheets>
     <sheet name="Biochamps MSP" sheetId="1" r:id="rId1"/>
@@ -4041,11 +4041,11 @@
   </sheetPr>
   <dimension ref="A1:AO110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13513,12 +13513,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96165BFD-25F4-48D7-9F9E-0D661328E082}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="O4" sqref="O4"/>
       <selection pane="topRight" activeCell="O4" sqref="O4"/>
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14624,7 +14624,7 @@
       <selection activeCell="O4" sqref="O4"/>
       <selection pane="topRight" activeCell="O4" sqref="O4"/>
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Palettisation model and schema, enhance Article model with PCB field, and update import process to handle palettisation data
</commit_message>
<xml_diff>
--- a/RESSOURCES/EMBALLAGES PAR PRODUITS TTES MARQUES.xlsx
+++ b/RESSOURCES/EMBALLAGES PAR PRODUITS TTES MARQUES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\econte\Desktop\Edouard\Divisio\RESSOURCES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367F2248-C3D9-4C2A-ACC0-5B57B79E029C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A6C752-33D0-4788-A921-D1B1531E8A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE562C63-56AB-4767-B83C-50F8A455B02C}"/>
   </bookViews>
@@ -4045,7 +4045,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10710,16 +10710,16 @@
   </sheetData>
   <autoFilter ref="J3:J18" xr:uid="{8FF0F9D2-17B0-4D09-9DF1-2E903DE4C1A8}"/>
   <mergeCells count="10">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:T2"/>
     <mergeCell ref="AC2:AE2"/>
     <mergeCell ref="AF2:AH2"/>
     <mergeCell ref="AI2:AO2"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="U2:X2"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" fitToWidth="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -10734,7 +10734,7 @@
   <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="O4" sqref="O4"/>
       <selection pane="topRight" activeCell="O4" sqref="O4"/>
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>

</xml_diff>

<commit_message>
Add CaracteristiqueArticle model and schema, enhance Article model with new relationship, and update import process to include characteristic data
</commit_message>
<xml_diff>
--- a/RESSOURCES/EMBALLAGES PAR PRODUITS TTES MARQUES.xlsx
+++ b/RESSOURCES/EMBALLAGES PAR PRODUITS TTES MARQUES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\econte\Desktop\Edouard\Divisio\RESSOURCES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A6C752-33D0-4788-A921-D1B1531E8A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A83529-0670-4CC1-AE33-BE22D4D9E376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE562C63-56AB-4767-B83C-50F8A455B02C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{CE562C63-56AB-4767-B83C-50F8A455B02C}"/>
   </bookViews>
   <sheets>
     <sheet name="Biochamps MSP" sheetId="1" r:id="rId1"/>
@@ -4041,11 +4041,11 @@
   </sheetPr>
   <dimension ref="A1:AO110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10710,16 +10710,16 @@
   </sheetData>
   <autoFilter ref="J3:J18" xr:uid="{8FF0F9D2-17B0-4D09-9DF1-2E903DE4C1A8}"/>
   <mergeCells count="10">
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AO2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="U2:X2"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="U2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" fitToWidth="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -13513,12 +13513,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96165BFD-25F4-48D7-9F9E-0D661328E082}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="O4" sqref="O4"/>
       <selection pane="topRight" activeCell="O4" sqref="O4"/>
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
-      <selection pane="bottomRight" activeCell="V4" sqref="V4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>